<commit_message>
send daily & weekly
</commit_message>
<xml_diff>
--- a/public/import/daily_template.xlsx
+++ b/public/import/daily_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -30,94 +30,31 @@
     <t>time</t>
   </si>
   <si>
-    <t>2023-05-29</t>
-  </si>
-  <si>
     <t>08:00</t>
   </si>
   <si>
-    <t>2023-06-01</t>
-  </si>
-  <si>
-    <t>2023-06-02</t>
-  </si>
-  <si>
-    <t>2023-06-03</t>
-  </si>
-  <si>
-    <t>2023-06-04</t>
-  </si>
-  <si>
     <t>10:00</t>
   </si>
   <si>
     <t>09:00</t>
   </si>
   <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>09:30</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>contoh task arik 1</t>
-  </si>
-  <si>
-    <t>contoh task arik 2</t>
-  </si>
-  <si>
-    <t>contoh task arik 3</t>
-  </si>
-  <si>
-    <t>contoh task arik 4</t>
-  </si>
-  <si>
-    <t>contoh task arik 5</t>
-  </si>
-  <si>
-    <t>contoh task arik 6</t>
-  </si>
-  <si>
-    <t>contoh task arik 7</t>
-  </si>
-  <si>
-    <t>contoh task arik 8</t>
-  </si>
-  <si>
-    <t>contoh task arik 9</t>
-  </si>
-  <si>
-    <t>contoh task arik 10</t>
-  </si>
-  <si>
-    <t>contoh task arik 11</t>
-  </si>
-  <si>
-    <t>contoh task arik 12</t>
-  </si>
-  <si>
-    <t>contoh task arik 13</t>
-  </si>
-  <si>
-    <t>contoh task arik 14</t>
-  </si>
-  <si>
-    <t>contoh task arik 15</t>
-  </si>
-  <si>
-    <t>contoh task arik 16</t>
-  </si>
-  <si>
-    <t>contoh task arik 17</t>
+    <t>2023-06-08</t>
+  </si>
+  <si>
+    <t>2023-06-09</t>
+  </si>
+  <si>
+    <t>contoh task import 1</t>
+  </si>
+  <si>
+    <t>contoh task import 2</t>
+  </si>
+  <si>
+    <t>contoh task import 3</t>
+  </si>
+  <si>
+    <t>contoh task import 4</t>
   </si>
 </sst>
 </file>
@@ -458,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,189 +421,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisi send daily&weekly, added by
</commit_message>
<xml_diff>
--- a/public/import/daily_template.xlsx
+++ b/public/import/daily_template.xlsx
@@ -39,12 +39,6 @@
     <t>09:00</t>
   </si>
   <si>
-    <t>2023-06-08</t>
-  </si>
-  <si>
-    <t>2023-06-09</t>
-  </si>
-  <si>
     <t>contoh task import 1</t>
   </si>
   <si>
@@ -55,6 +49,12 @@
   </si>
   <si>
     <t>contoh task import 4</t>
+  </si>
+  <si>
+    <t>2023-06-12</t>
+  </si>
+  <si>
+    <t>2023-06-13</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,10 +421,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -432,10 +432,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -443,10 +443,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Input KPI add 5 days
</commit_message>
<xml_diff>
--- a/public/import/daily_template.xlsx
+++ b/public/import/daily_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>date</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Review To Do List</t>
   </si>
   <si>
-    <t>15:00</t>
-  </si>
-  <si>
     <t>Morning briefing Retail</t>
   </si>
   <si>
@@ -58,96 +55,87 @@
     <t xml:space="preserve">Review To Do List </t>
   </si>
   <si>
-    <t xml:space="preserve">LPJ Coordinator Internal Audit </t>
-  </si>
-  <si>
     <t>Meeting Kospin SMS</t>
   </si>
   <si>
-    <t xml:space="preserve">14:00 </t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>Perjalanan ke Jakarta</t>
-  </si>
-  <si>
-    <t>Review achievement AMPM/KPI To Do List &amp; Do &amp; Done week 40</t>
-  </si>
-  <si>
-    <t>Create AMPM/To Do List Teddy</t>
-  </si>
-  <si>
     <t>13:00</t>
   </si>
   <si>
-    <t>Stock opname Gudang MMI Prima Center</t>
-  </si>
-  <si>
-    <t>Penelusuran selisih Trenly Tambun</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>Review LHP week 40</t>
-  </si>
-  <si>
-    <t>2023-10-09</t>
-  </si>
-  <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
-    <t>Review audit CV Maju Technology dengan Joe di Ocean Space</t>
-  </si>
-  <si>
-    <t>Review audit CCTV &amp; audit konsumen dengan Eni di Ocean Space</t>
-  </si>
-  <si>
-    <t>2023-10-11</t>
-  </si>
-  <si>
-    <t>Review finding status dengan Faizal &amp; Lula</t>
-  </si>
-  <si>
-    <t>appraisal dengan Fajar di CS</t>
-  </si>
-  <si>
-    <t>Review Telemarketing</t>
-  </si>
-  <si>
-    <t>Review audit Dolphin dengan Ridwan</t>
-  </si>
-  <si>
-    <t>LHP week 40</t>
-  </si>
-  <si>
-    <t>2023-10-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meeting CV SMJ </t>
-  </si>
-  <si>
-    <t>2023-10-13</t>
-  </si>
-  <si>
-    <t>Upgrade skill audit CV CS</t>
-  </si>
-  <si>
-    <t>2023-10-14</t>
+    <t>Review LHP week 44</t>
+  </si>
+  <si>
+    <t>Review achievement AMPM/KPI To Do List &amp; Do &amp; Done week 45</t>
+  </si>
+  <si>
+    <t>Create AMPM week 46</t>
+  </si>
+  <si>
+    <t>Review hasil stock opname Gudang PT MMI &amp; selisih setoran Trenly Tambun</t>
+  </si>
+  <si>
+    <t>Review audit SMJ: fisik SHM (covernote), berkas kredit (NAP)</t>
+  </si>
+  <si>
+    <t>Sharing session Audit, Verifikasi &amp; Investigasi di Kospin SMS</t>
+  </si>
+  <si>
+    <t>Review visit outlet distribution sales</t>
+  </si>
+  <si>
+    <t>LPJ Coordinator Audit (via Google Meet)</t>
+  </si>
+  <si>
+    <t>Review realisasi bundling, buku customer, buku COD</t>
+  </si>
+  <si>
+    <t>Review audit CV Maju Technology (via Google Meet)</t>
+  </si>
+  <si>
+    <t>Izin rontgent</t>
+  </si>
+  <si>
+    <t>Cuti Bersama Manager</t>
+  </si>
+  <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visit &amp; review AutoEV </t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review koreksi stok &amp; cashback toko retail </t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-17</t>
+  </si>
+  <si>
+    <t>2023-11-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,9 +158,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,304 +490,250 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
+      <c r="A2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
+      <c r="A5" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
+      <c r="A6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
+      <c r="A7" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
+      <c r="A8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>36</v>
+      <c r="A16" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
+      <c r="A17" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>38</v>
+      <c r="A22" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>